<commit_message>
Fixed bugs - calculation assetMarketAmount, equity and acquisition amounts correctly during a transfer.
</commit_message>
<xml_diff>
--- a/tests/Feature/config/mortgage_realistic.xlsx
+++ b/tests/Feature/config/mortgage_realistic.xlsx
@@ -2240,10 +2240,10 @@
       </c>
       <c r="AF19" s="9"/>
       <c r="AG19" s="8">
-        <v>-212712.0</v>
+        <v>-242869.0</v>
       </c>
       <c r="AH19" s="8">
-        <v>-420714.0</v>
+        <v>-450871.0</v>
       </c>
       <c r="AI19" s="9"/>
       <c r="AJ19" s="8">
@@ -2335,10 +2335,10 @@
       </c>
       <c r="AF20" s="2"/>
       <c r="AG20" s="1">
-        <v>-208979.6</v>
+        <v>-229504.6</v>
       </c>
       <c r="AH20" s="1">
-        <v>-629693.6</v>
+        <v>-680375.6</v>
       </c>
       <c r="AI20" s="2"/>
       <c r="AJ20" s="1">
@@ -2430,10 +2430,10 @@
       </c>
       <c r="AF21" s="2"/>
       <c r="AG21" s="1">
-        <v>-205709.58</v>
+        <v>-218779.58</v>
       </c>
       <c r="AH21" s="1">
-        <v>-835403.18</v>
+        <v>-899155.18</v>
       </c>
       <c r="AI21" s="2"/>
       <c r="AJ21" s="1">
@@ -2525,10 +2525,10 @@
       </c>
       <c r="AF22" s="2"/>
       <c r="AG22" s="1">
-        <v>-202902.759</v>
+        <v>-208903.759</v>
       </c>
       <c r="AH22" s="1">
-        <v>-1038305.939</v>
+        <v>-1108058.939</v>
       </c>
       <c r="AI22" s="2"/>
       <c r="AJ22" s="1">
@@ -2620,10 +2620,10 @@
       </c>
       <c r="AF23" s="2"/>
       <c r="AG23" s="1">
-        <v>-197856.998</v>
+        <v>-194064.998</v>
       </c>
       <c r="AH23" s="1">
-        <v>-1236162.937</v>
+        <v>-1302123.937</v>
       </c>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="1">
@@ -2715,10 +2715,10 @@
       </c>
       <c r="AF24" s="2"/>
       <c r="AG24" s="1">
-        <v>-198255.1979</v>
+        <v>-154856.1979</v>
       </c>
       <c r="AH24" s="1">
-        <v>-1434418.1349</v>
+        <v>-1456980.1349</v>
       </c>
       <c r="AI24" s="2"/>
       <c r="AJ24" s="1">
@@ -2810,10 +2810,10 @@
       </c>
       <c r="AF25" s="2"/>
       <c r="AG25" s="1">
-        <v>-198673.3079</v>
+        <v>-103297.3079</v>
       </c>
       <c r="AH25" s="1">
-        <v>-1633091.4428</v>
+        <v>-1560277.4428</v>
       </c>
       <c r="AI25" s="2"/>
       <c r="AJ25" s="1">
@@ -2905,10 +2905,10 @@
       </c>
       <c r="AF26" s="2"/>
       <c r="AG26" s="1">
-        <v>-67919.3234</v>
+        <v>-31661.3234</v>
       </c>
       <c r="AH26" s="1">
-        <v>-1701010.7662</v>
+        <v>-1591938.7662</v>
       </c>
       <c r="AI26" s="2"/>
       <c r="AJ26" s="1">
@@ -3003,7 +3003,7 @@
         <v>9379.7098</v>
       </c>
       <c r="AH27" s="1">
-        <v>-1691631.0564</v>
+        <v>-1582559.0564</v>
       </c>
       <c r="AI27" s="2"/>
       <c r="AJ27" s="1">
@@ -3098,7 +3098,7 @@
         <v>204746.6955</v>
       </c>
       <c r="AH28" s="1">
-        <v>-1486884.3609</v>
+        <v>-1377812.3609</v>
       </c>
       <c r="AI28" s="2"/>
       <c r="AJ28" s="1">
@@ -3193,7 +3193,7 @@
         <v>208159.4808</v>
       </c>
       <c r="AH29" s="1">
-        <v>-1278724.8801</v>
+        <v>-1169652.8801</v>
       </c>
       <c r="AI29" s="2"/>
       <c r="AJ29" s="1">
@@ -3288,7 +3288,7 @@
         <v>211610.854</v>
       </c>
       <c r="AH30" s="1">
-        <v>-1067114.0261</v>
+        <v>-958042.0261</v>
       </c>
       <c r="AI30" s="2"/>
       <c r="AJ30" s="1">
@@ -3383,7 +3383,7 @@
         <v>215099.5467</v>
       </c>
       <c r="AH31" s="1">
-        <v>-852014.4794</v>
+        <v>-742942.4794</v>
       </c>
       <c r="AI31" s="2"/>
       <c r="AJ31" s="1">
@@ -3478,7 +3478,7 @@
         <v>218625.2233</v>
       </c>
       <c r="AH32" s="1">
-        <v>-633389.2561</v>
+        <v>-524317.2561</v>
       </c>
       <c r="AI32" s="2"/>
       <c r="AJ32" s="1">
@@ -3573,7 +3573,7 @@
         <v>222187.4852</v>
       </c>
       <c r="AH33" s="1">
-        <v>-411201.7709</v>
+        <v>-302129.7709</v>
       </c>
       <c r="AI33" s="2"/>
       <c r="AJ33" s="1">
@@ -3668,7 +3668,7 @@
         <v>225782.8603</v>
       </c>
       <c r="AH34" s="1">
-        <v>-185418.9106</v>
+        <v>-76346.9106</v>
       </c>
       <c r="AI34" s="2"/>
       <c r="AJ34" s="1">
@@ -3763,7 +3763,7 @@
         <v>229387.378</v>
       </c>
       <c r="AH35" s="1">
-        <v>43968.4674</v>
+        <v>153040.4674</v>
       </c>
       <c r="AI35" s="2"/>
       <c r="AJ35" s="1">
@@ -3858,7 +3858,7 @@
         <v>232008.9446</v>
       </c>
       <c r="AH36" s="1">
-        <v>275977.412</v>
+        <v>385049.412</v>
       </c>
       <c r="AI36" s="2"/>
       <c r="AJ36" s="1">
@@ -3953,7 +3953,7 @@
         <v>233948.1916</v>
       </c>
       <c r="AH37" s="1">
-        <v>509925.6036</v>
+        <v>618997.6036</v>
       </c>
       <c r="AI37" s="2"/>
       <c r="AJ37" s="1">
@@ -4048,7 +4048,7 @@
         <v>235831.1998</v>
       </c>
       <c r="AH38" s="5">
-        <v>745756.8034</v>
+        <v>854828.8034</v>
       </c>
       <c r="AI38" s="16"/>
       <c r="AJ38" s="5">
@@ -6916,10 +6916,10 @@
       </c>
       <c r="AF19" s="9"/>
       <c r="AG19" s="8">
-        <v>0.0</v>
+        <v>-30157</v>
       </c>
       <c r="AH19" s="8">
-        <v>0.0</v>
+        <v>-30157.0</v>
       </c>
       <c r="AI19" s="9">
         <v>0.46294766666667</v>
@@ -7029,10 +7029,10 @@
       </c>
       <c r="AF20" s="2"/>
       <c r="AG20" s="1">
-        <v>0.0</v>
+        <v>-20525</v>
       </c>
       <c r="AH20" s="1">
-        <v>0.0</v>
+        <v>-50682.0</v>
       </c>
       <c r="AI20" s="2">
         <v>0.40253428571429</v>
@@ -7142,10 +7142,10 @@
       </c>
       <c r="AF21" s="2"/>
       <c r="AG21" s="1">
-        <v>0.0</v>
+        <v>-13070</v>
       </c>
       <c r="AH21" s="1">
-        <v>0.0</v>
+        <v>-63752.0</v>
       </c>
       <c r="AI21" s="2">
         <v>0.3439313681028</v>
@@ -7255,10 +7255,10 @@
       </c>
       <c r="AF22" s="2"/>
       <c r="AG22" s="1">
-        <v>0.0</v>
+        <v>-6001</v>
       </c>
       <c r="AH22" s="1">
-        <v>0.0</v>
+        <v>-69753.0</v>
       </c>
       <c r="AI22" s="2">
         <v>0.28732361516035</v>
@@ -7368,10 +7368,10 @@
       </c>
       <c r="AF23" s="2"/>
       <c r="AG23" s="1">
-        <v>0</v>
+        <v>3792</v>
       </c>
       <c r="AH23" s="1">
-        <v>0.0</v>
+        <v>-65961.0</v>
       </c>
       <c r="AI23" s="2">
         <v>0.23238683248325</v>
@@ -7481,10 +7481,10 @@
       </c>
       <c r="AF24" s="2"/>
       <c r="AG24" s="1">
-        <v>0</v>
+        <v>43399</v>
       </c>
       <c r="AH24" s="1">
-        <v>0.0</v>
+        <v>-22562.0</v>
       </c>
       <c r="AI24" s="2">
         <v>0.14633368548479</v>
@@ -7594,10 +7594,10 @@
       </c>
       <c r="AF25" s="2"/>
       <c r="AG25" s="1">
-        <v>0</v>
+        <v>95376</v>
       </c>
       <c r="AH25" s="1">
-        <v>0.0</v>
+        <v>72814.0</v>
       </c>
       <c r="AI25" s="2">
         <v>0.073202982772125</v>
@@ -7707,10 +7707,10 @@
       </c>
       <c r="AF26" s="2"/>
       <c r="AG26" s="1">
-        <v>131193.0</v>
+        <v>167451</v>
       </c>
       <c r="AH26" s="1">
-        <v>131193.0</v>
+        <v>240265.0</v>
       </c>
       <c r="AI26" s="2">
         <v>0.016848123362916</v>
@@ -7806,10 +7806,10 @@
       </c>
       <c r="AF27" s="2"/>
       <c r="AG27" s="1">
-        <v>208953.0</v>
+        <v>208953</v>
       </c>
       <c r="AH27" s="1">
-        <v>340146.0</v>
+        <v>449218.0</v>
       </c>
       <c r="AI27" s="2"/>
       <c r="AJ27" s="1">
@@ -7901,10 +7901,10 @@
       </c>
       <c r="AF28" s="2"/>
       <c r="AG28" s="1">
-        <v>212811.0</v>
+        <v>212811</v>
       </c>
       <c r="AH28" s="1">
-        <v>552957.0</v>
+        <v>662029.0</v>
       </c>
       <c r="AI28" s="2"/>
       <c r="AJ28" s="1">
@@ -7996,10 +7996,10 @@
       </c>
       <c r="AF29" s="2"/>
       <c r="AG29" s="1">
-        <v>216732.0</v>
+        <v>216732</v>
       </c>
       <c r="AH29" s="1">
-        <v>769689.0</v>
+        <v>878761.0</v>
       </c>
       <c r="AI29" s="2"/>
       <c r="AJ29" s="1">
@@ -8091,10 +8091,10 @@
       </c>
       <c r="AF30" s="2"/>
       <c r="AG30" s="1">
-        <v>220717.0</v>
+        <v>220717</v>
       </c>
       <c r="AH30" s="1">
-        <v>990406.0</v>
+        <v>1099478.0</v>
       </c>
       <c r="AI30" s="2"/>
       <c r="AJ30" s="1">
@@ -8186,10 +8186,10 @@
       </c>
       <c r="AF31" s="2"/>
       <c r="AG31" s="1">
-        <v>224766.0</v>
+        <v>224766</v>
       </c>
       <c r="AH31" s="1">
-        <v>1215172.0</v>
+        <v>1324244.0</v>
       </c>
       <c r="AI31" s="2"/>
       <c r="AJ31" s="1">
@@ -8281,10 +8281,10 @@
       </c>
       <c r="AF32" s="2"/>
       <c r="AG32" s="1">
-        <v>228880.0</v>
+        <v>228880</v>
       </c>
       <c r="AH32" s="1">
-        <v>1444052.0</v>
+        <v>1553124.0</v>
       </c>
       <c r="AI32" s="2"/>
       <c r="AJ32" s="1">
@@ -8376,10 +8376,10 @@
       </c>
       <c r="AF33" s="2"/>
       <c r="AG33" s="1">
-        <v>233060.0</v>
+        <v>233060</v>
       </c>
       <c r="AH33" s="1">
-        <v>1677112.0</v>
+        <v>1786184.0</v>
       </c>
       <c r="AI33" s="2"/>
       <c r="AJ33" s="1">
@@ -8471,10 +8471,10 @@
       </c>
       <c r="AF34" s="2"/>
       <c r="AG34" s="1">
-        <v>237304.0</v>
+        <v>237304</v>
       </c>
       <c r="AH34" s="1">
-        <v>1914416.0</v>
+        <v>2023488.0</v>
       </c>
       <c r="AI34" s="2"/>
       <c r="AJ34" s="1">
@@ -8566,10 +8566,10 @@
       </c>
       <c r="AF35" s="2"/>
       <c r="AG35" s="1">
-        <v>241616.0</v>
+        <v>241616</v>
       </c>
       <c r="AH35" s="1">
-        <v>2156032.0</v>
+        <v>2265104.0</v>
       </c>
       <c r="AI35" s="2"/>
       <c r="AJ35" s="1">
@@ -8661,10 +8661,10 @@
       </c>
       <c r="AF36" s="2"/>
       <c r="AG36" s="1">
-        <v>245804.0</v>
+        <v>245804</v>
       </c>
       <c r="AH36" s="1">
-        <v>2401836.0</v>
+        <v>2510908.0</v>
       </c>
       <c r="AI36" s="2"/>
       <c r="AJ36" s="1">
@@ -8756,10 +8756,10 @@
       </c>
       <c r="AF37" s="2"/>
       <c r="AG37" s="1">
-        <v>249388.0</v>
+        <v>249388</v>
       </c>
       <c r="AH37" s="1">
-        <v>2651224.0</v>
+        <v>2760296.0</v>
       </c>
       <c r="AI37" s="2"/>
       <c r="AJ37" s="1">
@@ -8851,10 +8851,10 @@
       </c>
       <c r="AF38" s="16"/>
       <c r="AG38" s="5">
-        <v>252998.0</v>
+        <v>252998</v>
       </c>
       <c r="AH38" s="5">
-        <v>2904222.0</v>
+        <v>3013294.0</v>
       </c>
       <c r="AI38" s="16"/>
       <c r="AJ38" s="5">

</xml_diff>